<commit_message>
affichage coups grille pas fini
</commit_message>
<xml_diff>
--- a/Journaux/JournalDeTravail.xlsx
+++ b/Journaux/JournalDeTravail.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="106">
   <si>
     <t>Date</t>
   </si>
@@ -324,6 +324,33 @@
   </si>
   <si>
     <t>J'ai comencé la maquete</t>
+  </si>
+  <si>
+    <t>J'ai transformer la lettre de la colonne en numéro(ex.: A = 1)</t>
+  </si>
+  <si>
+    <t>M. Viret https://www.google.com/search?q=ascii+table&amp;rlz=1C1PNJJ_frCH968CH968&amp;source=lnms&amp;tbm=isch&amp;sa=X&amp;ved=2ahUKEwjB0t_xsqn2AhURP-wKHZtWAAIQ_AUoAXoECAEQAw&amp;biw=1744&amp;bih=917&amp;dpr=1.1#imgrc=P0o7oyvJKm4ETM</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/1469711/converting-letters-to-numbers-in-c</t>
+  </si>
+  <si>
+    <t>J'ai commenter ma fonction ColumnNumber</t>
+  </si>
+  <si>
+    <t>Affichage des coups dans la grille</t>
+  </si>
+  <si>
+    <t>J'ai comencé la fonction qui affiche les coups dans la grille</t>
+  </si>
+  <si>
+    <t>J'ai fini la fonction qui affiche les coups sur la grille. Ça ne marche pas</t>
+  </si>
+  <si>
+    <t>J'ai comencé à débugger ma fonction qui affiche les coups sur la grille</t>
+  </si>
+  <si>
+    <t>Romain</t>
   </si>
 </sst>
 </file>
@@ -845,7 +872,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H61" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H66" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
   <tableColumns count="8">
     <tableColumn id="1" name="Date" dataDxfId="16"/>
     <tableColumn id="2" name="Heure début" dataDxfId="15"/>
@@ -1125,10 +1152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,7 +2421,7 @@
       <c r="G49" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H49" s="5" t="s">
+      <c r="H49" s="35" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2527,7 +2554,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16">
         <v>44622</v>
       </c>
@@ -2551,7 +2578,7 @@
         <v>87</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2705,6 +2732,133 @@
         <v>96</v>
       </c>
       <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="21">
+        <v>44623</v>
+      </c>
+      <c r="B62" s="24">
+        <v>0.34375</v>
+      </c>
+      <c r="C62" s="24">
+        <v>0.36041666666666666</v>
+      </c>
+      <c r="D62" s="20">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>1.6666666666666663E-2</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="16">
+        <v>44623</v>
+      </c>
+      <c r="B63" s="19">
+        <v>0.36249999999999999</v>
+      </c>
+      <c r="C63" s="19">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="D63" s="18">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>3.4722222222222099E-3</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="21">
+        <v>44623</v>
+      </c>
+      <c r="B64" s="24">
+        <v>0.3666666666666667</v>
+      </c>
+      <c r="C64" s="24">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="D64" s="20">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>3.2638888888888884E-2</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="21">
+        <v>44623</v>
+      </c>
+      <c r="B65" s="24">
+        <v>0.41875000000000001</v>
+      </c>
+      <c r="C65" s="24">
+        <v>0.44236111111111115</v>
+      </c>
+      <c r="D65" s="20">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>2.3611111111111138E-2</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="16">
+        <v>44623</v>
+      </c>
+      <c r="B66" s="19">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="C66" s="19"/>
+      <c r="D66" s="18">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>-0.44444444444444442</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>105</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
@@ -2720,7 +2874,7 @@
       <formula>NOT(ISERROR(SEARCH("Date",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D220:D1048576 D1:D193">
+  <conditionalFormatting sqref="D223:D1048576 D1:D196">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
       <formula>0.0833</formula>
     </cfRule>
@@ -2753,11 +2907,12 @@
     <hyperlink ref="H33" r:id="rId2"/>
     <hyperlink ref="H34" r:id="rId3"/>
     <hyperlink ref="H36" r:id="rId4"/>
+    <hyperlink ref="H49" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lire la carte réussi
</commit_message>
<xml_diff>
--- a/Journaux/JournalDeTravail.xlsx
+++ b/Journaux/JournalDeTravail.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="124">
   <si>
     <t>Date</t>
   </si>
@@ -401,6 +400,12 @@
   </si>
   <si>
     <t>M. Wyssa</t>
+  </si>
+  <si>
+    <t>Créer les 5 grilles</t>
+  </si>
+  <si>
+    <t>M. Viret m'a expliqué et aidé sur Teams comment lire un fichier. J'ai donc plus de problèmes</t>
   </si>
 </sst>
 </file>
@@ -922,7 +927,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H76" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H77" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
   <tableColumns count="8">
     <tableColumn id="1" name="Date" dataDxfId="16"/>
     <tableColumn id="2" name="Heure début" dataDxfId="15"/>
@@ -1202,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+      <selection activeCell="H77" sqref="H77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3168,6 +3173,33 @@
         <v>121</v>
       </c>
     </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="21">
+        <v>44638</v>
+      </c>
+      <c r="B77" s="24">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="C77" s="24">
+        <v>0.62430555555555556</v>
+      </c>
+      <c r="D77" s="20">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>2.7083333333333348E-2</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H77" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
@@ -3182,7 +3214,7 @@
       <formula>NOT(ISERROR(SEARCH("Date",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D232:D1048576 D1:D205">
+  <conditionalFormatting sqref="D233:D1048576 D1:D206">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
       <formula>0.0833</formula>
     </cfRule>

</xml_diff>

<commit_message>
diagramme de flux début
</commit_message>
<xml_diff>
--- a/Journaux/JournalDeTravail.xlsx
+++ b/Journaux/JournalDeTravail.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="155">
   <si>
     <t>Date</t>
   </si>
@@ -490,6 +490,15 @@
   </si>
   <si>
     <t>J'ai fait le MCD</t>
+  </si>
+  <si>
+    <t>Diagramme de flux</t>
+  </si>
+  <si>
+    <t>J'ai commencé le diagramme de flux</t>
+  </si>
+  <si>
+    <t>J'ai continué le diagramme de flux</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1020,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H94" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau4" displayName="Tableau4" ref="A1:H96" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18">
   <tableColumns count="8">
     <tableColumn id="1" name="Date" dataDxfId="16"/>
     <tableColumn id="2" name="Heure début" dataDxfId="15"/>
@@ -1291,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L76" sqref="L76"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3719,6 +3728,56 @@
       </c>
       <c r="H94" s="5"/>
     </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="21">
+        <v>44652</v>
+      </c>
+      <c r="B95" s="24">
+        <v>0.73611111111111116</v>
+      </c>
+      <c r="C95" s="24">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D95" s="20">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>3.472222222222221E-2</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G95" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="H95" s="5"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="21">
+        <v>44652</v>
+      </c>
+      <c r="B96" s="24">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="C96" s="24">
+        <v>0.62430555555555556</v>
+      </c>
+      <c r="D96" s="20">
+        <f>Tableau4[[#This Row],[Heure fin]]-Tableau4[[#This Row],[Heure début]]</f>
+        <v>3.4027777777777768E-2</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G96" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H96" s="5"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="greaterThan">
@@ -3733,7 +3792,7 @@
       <formula>NOT(ISERROR(SEARCH("Date",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D248:D1048576 D1:D221">
+  <conditionalFormatting sqref="D250:D1048576 D1:D223">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThanOrEqual">
       <formula>0.0833</formula>
     </cfRule>

</xml_diff>